<commit_message>
fix: remove checkbox for reconciling a transaction and update UI functions
</commit_message>
<xml_diff>
--- a/data/transactions.xlsx
+++ b/data/transactions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,18 +451,216 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Type</t>
+          <t>Debit</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Amount</t>
+          <t>Credit</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Balance</t>
         </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Reconciled</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2/9/25</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>paycheck</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>me</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>400</v>
+      </c>
+      <c r="F2" t="n">
+        <v>400</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2/9/25</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Bar Tab</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Some Watering Hole</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>30</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>370</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2/9/25</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Dinner</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Slim Chicken</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>25.69</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>344.31</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2/9/25</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Chime Transfer</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Chime</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>244.31</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-03-01</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Starting Balance</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>244.31</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2/10/25</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Some Description</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>A Payee</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>8</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>236.31</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>3/10/25</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Some Description</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>A Payee</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>8</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>228.31</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>